<commit_message>
Vertabanı raporu ve tablosu güncellendi
</commit_message>
<xml_diff>
--- a/docs/Veri Tabanı Tabloları.xlsx
+++ b/docs/Veri Tabanı Tabloları.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bera\Desktop\mucizeOl\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D90B7C3-63A5-4B49-BB60-1D7ED8BFF9DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96C4E16E-633B-48B4-AD3A-F69465F934AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{20C72D80-65A9-4621-989B-3A9B5B557A8B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
   <si>
     <t>password_hash</t>
   </si>
@@ -74,18 +74,6 @@
     <t>role_name</t>
   </si>
   <si>
-    <t xml:space="preserve">user_refresh_tokens </t>
-  </si>
-  <si>
-    <t>token_id</t>
-  </si>
-  <si>
-    <t>token_hash</t>
-  </si>
-  <si>
-    <t>expires_at</t>
-  </si>
-  <si>
     <t xml:space="preserve">listings </t>
   </si>
   <si>
@@ -162,6 +150,12 @@
   </si>
   <si>
     <t>breed_name</t>
+  </si>
+  <si>
+    <t>refresh_token_hash</t>
+  </si>
+  <si>
+    <t>refresh_token_expires_at</t>
   </si>
 </sst>
 </file>
@@ -260,7 +254,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -273,14 +267,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -615,15 +610,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CFAE65F-F72C-4D34-A926-6D7A446A28C9}">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.77734375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.109375" bestFit="1" customWidth="1"/>
@@ -631,186 +626,174 @@
     <col min="9" max="9" width="11.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" thickBot="1">
+    <row r="1" spans="1:8" ht="15" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="E1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="15" thickBot="1">
+      <c r="E2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15" thickBot="1">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="15" thickBot="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15" thickBot="1">
+      <c r="A7" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="4" t="s">
+    <row r="8" spans="1:8" ht="15" thickBot="1">
+      <c r="A8" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15" thickBot="1">
+      <c r="A9" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="15" thickBot="1">
-      <c r="A8" s="4" t="s">
+      <c r="C9" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="6"/>
+      <c r="H9" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15" thickBot="1">
+      <c r="A10" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="15" thickBot="1">
-      <c r="A9" s="7" t="s">
+      <c r="C10" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15" thickBot="1">
+      <c r="A11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="G9" s="6"/>
-      <c r="H9" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="C10" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
       <c r="C11" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H11" s="10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="15" thickBot="1">
+      <c r="E11" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="C12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15" thickBot="1">
+      <c r="C13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="C14" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="C15" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="C16" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="C13" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="C14" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="15" thickBot="1">
-      <c r="C15" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="C16" s="4" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="17" spans="3:3">
       <c r="C17" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="3:3">
       <c r="C18" s="4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="3:3">
       <c r="C19" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="3:3">
       <c r="C20" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="3:3">
@@ -820,7 +803,7 @@
     </row>
     <row r="22" spans="3:3" ht="15" thickBot="1">
       <c r="C22" s="5" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>